<commit_message>
REFACTOR : Ajustes de test unitarios, cobertura y modificaciones de meetodos
</commit_message>
<xml_diff>
--- a/Documentación/Diccionario.xlsx
+++ b/Documentación/Diccionario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\OneDrive\Escritorio\Santiago\ORT\Diseño de Aplicaciones 2\Obligatorio1\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3E2AB4-69ED-4129-968B-1B2E944DCEAA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D58A4CC2-B966-4773-952B-31467EB5E33A}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13224" windowHeight="5748" xr2:uid="{D78A2918-D528-456C-B848-882338DF88B2}"/>
   </bookViews>
@@ -918,7 +918,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Fix al borrar sport con equipos
</commit_message>
<xml_diff>
--- a/Documentación/Diccionario.xlsx
+++ b/Documentación/Diccionario.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\OneDrive\Escritorio\Santiago\ORT\Diseño de Aplicaciones 2\Obligatorio1\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi_reaqng9\Desktop\ORT\DA2\Oblig1_DA2\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3E2AB4-69ED-4129-968B-1B2E944DCEAA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB9FF3A-2B83-47C5-A343-6FF8FEF9BEF6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13224" windowHeight="5748" xr2:uid="{D78A2918-D528-456C-B848-882338DF88B2}"/>
   </bookViews>
@@ -346,9 +346,6 @@
     <t>/api/team/{teamName}</t>
   </si>
   <si>
-    <t>DELETE DeleteTeamByUserName</t>
-  </si>
-  <si>
     <t>/api/sport/</t>
   </si>
   <si>
@@ -362,9 +359,6 @@
   </si>
   <si>
     <t>PUT ModifySportByName</t>
-  </si>
-  <si>
-    <t>DELETE DeleteSportByUserName</t>
   </si>
   <si>
     <t>/api/sport/{sportName}</t>
@@ -484,9 +478,6 @@
     <t>/api/user/{userName}</t>
   </si>
   <si>
-    <t>GET GetSportByUserName</t>
-  </si>
-  <si>
     <t>POST AddUserRequest</t>
   </si>
   <si>
@@ -515,12 +506,21 @@
   </si>
   <si>
     <t>Servicios adicionales</t>
+  </si>
+  <si>
+    <t>DELETE DeleteTeamByName</t>
+  </si>
+  <si>
+    <t>DELETE DeleteSportByName</t>
+  </si>
+  <si>
+    <t>GET GetSportByName</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -605,8 +605,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{A18B4719-305A-4B62-A3A7-9DC9308B8985}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -917,21 +945,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF250CE1-C621-4CE1-9619-C558EC965D5F}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="57.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.7890625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="92.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.89453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="92.89453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.89453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.89453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -948,7 +976,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -960,10 +988,10 @@
         <v>24</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -978,7 +1006,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -993,7 +1021,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -1008,7 +1036,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1023,7 +1051,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -1035,10 +1063,10 @@
         <v>34</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -1047,13 +1075,13 @@
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -1062,13 +1090,13 @@
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -1077,13 +1105,13 @@
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -1092,13 +1120,13 @@
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -1107,13 +1135,13 @@
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -1122,13 +1150,13 @@
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
@@ -1137,13 +1165,13 @@
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
@@ -1152,13 +1180,13 @@
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
@@ -1167,13 +1195,13 @@
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
@@ -1182,13 +1210,13 @@
         <v>22</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
@@ -1197,13 +1225,13 @@
         <v>22</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3" t="s">
         <v>19</v>
       </c>
@@ -1212,28 +1240,28 @@
         <v>22</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -1242,13 +1270,13 @@
         <v>22</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -1257,52 +1285,52 @@
         <v>22</v>
       </c>
       <c r="D22" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="B24" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D24" s="4" t="s">
+      <c r="E24" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
       <c r="D25" s="3" t="s">
         <v>28</v>
       </c>
@@ -1310,40 +1338,40 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="6"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
       <c r="D26" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="5"/>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="6"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
       <c r="D27" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="5"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
+        <v>69</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" s="6"/>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
       <c r="D28" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>

</xml_diff>

<commit_message>
Se agregan documento de obligatorio y diccionario de servicios ajustado.
</commit_message>
<xml_diff>
--- a/Documentación/Diccionario.xlsx
+++ b/Documentación/Diccionario.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi_reaqng9\Desktop\ORT\DA2\Oblig1_DA2\Documentación\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\santi\OneDrive\Escritorio\Santiago\ORT\Diseño de Aplicaciones 2\Obli1\Documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECB9FF3A-2B83-47C5-A343-6FF8FEF9BEF6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03619372-34C5-4F5B-A1E5-69B1F3A78A54}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13224" windowHeight="5748" xr2:uid="{D78A2918-D528-456C-B848-882338DF88B2}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="76">
   <si>
     <t>Administrador</t>
   </si>
@@ -558,7 +558,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -577,11 +577,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="dotted">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="dotted">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -598,7 +616,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -945,21 +969,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF250CE1-C621-4CE1-9619-C558EC965D5F}">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="57.7890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.77734375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.89453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="92.89453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.89453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.89453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="92.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -976,7 +1000,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -991,7 +1015,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1006,7 +1030,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -1021,7 +1045,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -1036,7 +1060,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1051,7 +1075,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -1066,7 +1090,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -1081,7 +1105,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -1096,7 +1120,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
@@ -1111,7 +1135,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
@@ -1126,7 +1150,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
@@ -1141,7 +1165,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -1156,7 +1180,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>15</v>
       </c>
@@ -1171,7 +1195,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>16</v>
       </c>
@@ -1186,7 +1210,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
@@ -1201,11 +1225,13 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="C17" s="3" t="s">
         <v>22</v>
       </c>
@@ -1216,11 +1242,13 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="C18" s="3" t="s">
         <v>22</v>
       </c>
@@ -1231,11 +1259,13 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="3"/>
+      <c r="B19" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="C19" s="3" t="s">
         <v>22</v>
       </c>
@@ -1246,11 +1276,13 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B20" s="3"/>
+      <c r="B20" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="C20" s="3" t="s">
         <v>22</v>
       </c>
@@ -1261,11 +1293,13 @@
         <v>56</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="3"/>
+      <c r="B21" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="C21" s="3" t="s">
         <v>22</v>
       </c>
@@ -1276,11 +1310,13 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="3"/>
+      <c r="B22" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="C22" s="3" t="s">
         <v>22</v>
       </c>
@@ -1291,7 +1327,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>62</v>
       </c>
@@ -1308,7 +1344,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>63</v>
       </c>
@@ -1325,12 +1361,16 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
+      <c r="B25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="D25" s="3" t="s">
         <v>28</v>
       </c>
@@ -1338,10 +1378,14 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="7"/>
+      <c r="B26" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="D26" s="3" t="s">
         <v>44</v>
       </c>
@@ -1349,10 +1393,14 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A27" s="6"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="7"/>
+      <c r="B27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="D27" s="3" t="s">
         <v>69</v>
       </c>
@@ -1360,10 +1408,14 @@
         <v>68</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A28" s="6"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="8"/>
+      <c r="B28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="D28" s="3" t="s">
         <v>40</v>
       </c>
@@ -1371,14 +1423,14 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A25:C28"/>
+    <mergeCell ref="A25:A28"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A17" r:id="rId1" location="heading=h.bhsgeuh6zrib" display="heading=h.bhsgeuh6zrib" xr:uid="{7A4373B6-2865-468C-A6E3-41FF535F7696}"/>

</xml_diff>